<commit_message>
add files, beginning of while loops
</commit_message>
<xml_diff>
--- a/Hangman_v4.xlsx
+++ b/Hangman_v4.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding\Projects\CodeCool\Projects\Week 3\Hangman_Team\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FAB7EB-59A0-4B7A-AEA5-57FE6C43BC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD28807-65DC-4F61-BC5B-B647B7200150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25710" yWindow="-110" windowWidth="25820" windowHeight="15620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>Ha olyan betut ir be ami nem szerepel a szoban, akkor le kell vonni 1 eletet</t>
   </si>
@@ -133,6 +134,45 @@
   </si>
   <si>
     <t>addToArrayUserWorking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int userChoice = </t>
+  </si>
+  <si>
+    <t>Case 1</t>
+  </si>
+  <si>
+    <t>eletek</t>
+  </si>
+  <si>
+    <t>Case 2</t>
+  </si>
+  <si>
+    <t>hos</t>
+  </si>
+  <si>
+    <t>Cas 3</t>
+  </si>
+  <si>
+    <t>userArray</t>
+  </si>
+  <si>
+    <t>initalArray</t>
+  </si>
+  <si>
+    <t>Array Nehez</t>
+  </si>
+  <si>
+    <t>Array kozepes</t>
+  </si>
+  <si>
+    <t>Array konntu</t>
+  </si>
+  <si>
+    <t>u ArrayList&lt;String&gt; initialWordArray = createInitialWordArray(solutionArrayHard);</t>
+  </si>
+  <si>
+    <t>u ArrayList&lt;String&gt; initialWordArray = createInitialWordArray(solutionArrayMEdium)</t>
   </si>
 </sst>
 </file>
@@ -8274,6 +8314,216 @@
         </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>136525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8136ACD1-5334-38F8-F349-848A7951CBD6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3038475" y="596900"/>
+          <a:ext cx="1066800" cy="492125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Show Menu</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>530225</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>117475</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>377825</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>34925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBC203B2-9F53-4BF0-A509-85A08831C9BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2968625" y="1260475"/>
+          <a:ext cx="1066800" cy="679450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>getUserInput()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Scanner</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>return</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>149225</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Diamond 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C43E5D1-E310-643B-C194-E917CF3E2EB7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2641600" y="2244725"/>
+          <a:ext cx="952500" cy="1431925"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -8579,8 +8829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H95"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F87" sqref="F87"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8691,4 +8941,86 @@
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{172DF22D-C4BC-467B-8F82-F1D1A6695F4C}">
+  <dimension ref="D4:O24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="4:15" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>